<commit_message>
Redesign the bars and fix some bugs
- Change damage and health from float to int
- Balance tweak
- Fix early blinking on low health
</commit_message>
<xml_diff>
--- a/UnitStatus.xlsx
+++ b/UnitStatus.xlsx
@@ -158,7 +158,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>125+25+25</t>
+    <t>125+25+15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -524,7 +524,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adjust balance and fix bugs
- Change the font of boss name
- Nerf the health of enemies
- Nerf wave 1-3, 1-4
- Fix bug of Laser: isPiercing not work
- Mothership would destroy all remaining droids upon death
- Increase the exp of Cruisers
- Boltweapon would gain shots with larger angle first as upgrading
- Fix the bug that the boss health bar won't replenish
- Increase the duration of wave 3-4
</commit_message>
<xml_diff>
--- a/UnitStatus.xlsx
+++ b/UnitStatus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -769,7 +769,7 @@
         <v>33</v>
       </c>
       <c r="D12" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s">
         <v>38</v>
@@ -860,7 +860,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1">
         <v>25</v>
@@ -880,7 +880,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="1">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="C20" s="1">
         <v>50</v>
@@ -900,7 +900,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E21" s="1">
         <v>2.5000000000000001E-2</v>
@@ -917,7 +917,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1">
         <v>2.5000000000000001E-2</v>
@@ -934,7 +934,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1">
         <v>2.5000000000000001E-2</v>
@@ -951,7 +951,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1">
         <v>2.5000000000000001E-2</v>
@@ -968,7 +968,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="1">
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="E25" s="1">
         <v>0.05</v>
@@ -977,7 +977,7 @@
         <v>200</v>
       </c>
       <c r="G25" s="1">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -985,7 +985,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="1">
-        <v>960</v>
+        <v>800</v>
       </c>
       <c r="E26" s="1">
         <v>0.05</v>
@@ -994,7 +994,7 @@
         <v>500</v>
       </c>
       <c r="G26" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1002,7 +1002,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E27" s="1">
         <v>2.5000000000000001E-2</v>
@@ -1093,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="C4">
         <f>2*Status!G25 + 5*Status!G21</f>
-        <v>100</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1146,8 +1146,8 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <f>8*Status!G21 + 8*Status!G23</f>
-        <v>160</v>
+        <f>6*Status!G21 + 6*Status!G23</f>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1162,7 +1162,7 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7">
         <f>SUM(C2:C6)</f>
-        <v>426.66666666666669</v>
+        <v>416.66666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1174,7 +1174,7 @@
       </c>
       <c r="C8">
         <f>2*Status!G25 + 8*Status!G22</f>
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="C11">
         <f>4*Status!G25 + 12*Status!G23</f>
-        <v>220</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1216,7 +1216,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13">
         <f t="shared" ref="C13:C19" si="0">SUM(C8:C12)</f>
-        <v>733.33333333333337</v>
+        <v>823.33333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="C16">
         <f>3*Status!G26 + 12*Status!G24</f>
-        <v>270</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1270,7 +1270,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>1080</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="C20">
         <f>SUM(C7,C13,C19)</f>
-        <v>2240</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>